<commit_message>
Project code + updated expenses
I received the project code from Charmaine (there are mistakes - CD to fix)
Also, I updated CApelin_SPERA_Expenses.xlsx. In several cases I had included tax in the cost of purchases (tax should not be included). I updated the costs. We have ~3.2K in O&M to spend
</commit_message>
<xml_diff>
--- a/Capelin_SPERA_Expenses.xlsx
+++ b/Capelin_SPERA_Expenses.xlsx
@@ -120,7 +120,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +170,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -179,7 +191,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -261,11 +273,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -301,6 +328,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -606,7 +639,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,9 +707,8 @@
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8">
-        <f>+E8*D8</f>
-        <v>5500.35</v>
+      <c r="F8" s="15">
+        <v>4782.91</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -695,9 +727,8 @@
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9">
-        <f t="shared" ref="F9:F13" si="0">+E9*D9</f>
-        <v>126.48</v>
+      <c r="F9" s="14">
+        <v>109.98</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -717,8 +748,7 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
-        <v>701.73</v>
+        <v>610.20000000000005</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -738,7 +768,7 @@
         <v>1.66</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F9:F13" si="0">+E11*D11</f>
         <v>954.5</v>
       </c>
     </row>
@@ -790,7 +820,7 @@
       </c>
       <c r="F15" s="2">
         <f>SUM(F8:F13)</f>
-        <v>7652.0599999999995</v>
+        <v>6826.5899999999992</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -918,7 +948,7 @@
     <mergeCell ref="A20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>